<commit_message>
Added Decision Tree Algorithm
</commit_message>
<xml_diff>
--- a/hello.xlsx
+++ b/hello.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/willwen/anaconda3/envs/privacy_policy_tool/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2C2A0D3-45D3-D941-BDBA-45F7F3C9F1FC}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B60A43EF-D0D7-8343-852B-67CC54322116}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3180" yWindow="2060" windowWidth="27640" windowHeight="16940" xr2:uid="{A800D5BB-7C02-BC4D-8255-D4B05FAF7706}"/>
   </bookViews>
@@ -964,8 +964,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51EB194A-667F-D24F-A47B-83D2537A3165}">
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>